<commit_message>
Various things have been changed.
</commit_message>
<xml_diff>
--- a/old_project/Database/backup_data/Input_Backup.xlsx
+++ b/old_project/Database/backup_data/Input_Backup.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="New_Cases" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1668" uniqueCount="1192">
   <si>
     <t xml:space="preserve">Case Name</t>
   </si>
@@ -3086,6 +3086,535 @@
   </si>
   <si>
     <t xml:space="preserve">Note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harford v Morris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Hag Con 422</t>
+  </si>
+  <si>
+    <t xml:space="preserve">151 ER 792</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engri0161&amp;i=798</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Middleton v Janverin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Hag Con 436</t>
+  </si>
+  <si>
+    <t xml:space="preserve">161 ER 767</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engri0161&amp;i=803</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lex loci contractus, lex domicili</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campbell v Stein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 Dow PC 116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 ER 1417</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engra0003&amp;i=1425</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lacon v Higgins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dow &amp; Ryl NP 38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">171 ER 910</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrk0171&amp;i=914</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curling v Thornton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Add 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">162 ER 198</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engri0162&amp;i=202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beazley v Beazley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Hagg Ecc 639</t>
+  </si>
+  <si>
+    <t xml:space="preserve">162 ER 1292</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engri0162&amp;i=1296</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Houlditch v Marquess of Donegall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Cl &amp; Fin 470</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 ER 1232</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engra0006&amp;i=1244</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Woodham v Edwards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Ad &amp; E 771</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111 ER 1358</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrf0111&amp;i=1362</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brown v Thornton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 Ad &amp; E 185</t>
+  </si>
+  <si>
+    <t xml:space="preserve">112 ER 70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrf0112&amp;i=74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clark v Mullick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Moo 252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 ER 106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrb0013&amp;i=112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lex loci solutionis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Callandar v Dittrich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Man &amp; G 68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">134 ER 29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrg0134&amp;i=33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duncan v Campbell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 Sim 615</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59 ER 1269</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.engrep/engre0059&amp;i=1277</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Gibbs v Potter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 M&amp;W 70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">152 ER 386</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrh0152&amp;i=390</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mittelholzer v Fullarton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 QB 989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">115 ER 989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrf0115&amp;i=377</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hartley v Manton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 QB 247</t>
+  </si>
+  <si>
+    <t xml:space="preserve">114 ER 1242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrf0114&amp;i=1246</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La Constancia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 W Rob 487</t>
+  </si>
+  <si>
+    <t xml:space="preserve">166 ER 839</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engri0166&amp;i=843</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bain v Whitehaven and Furness Railway CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 HLC 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 ER 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engra0010&amp;i=13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonar v Mitchell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Ex 415</t>
+  </si>
+  <si>
+    <t xml:space="preserve">155 ER 181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrh0155&amp;i=185</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Segregdo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Sp Ecc &amp; Ad 36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">164 ER 22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engri0167&amp;i=253</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Este v Smyth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 Beav 112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52 ER 55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrd0052&amp;i=52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duncan v Canan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 De Ge M&amp;G 78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44 ER 31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrc0044&amp;i=37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cammell v Sewell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 H&amp;N 617</t>
+  </si>
+  <si>
+    <t xml:space="preserve">157 ER 615</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrh0157&amp;i=619</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cope v Doherty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 K&amp;J 367</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70 ER 154</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shipping </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engre0070&amp;i=160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Milford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swab 362</t>
+  </si>
+  <si>
+    <t xml:space="preserve">166 ER 1167</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engri0166&amp;i=1171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mette v Mette</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Sw &amp; Tr 416</t>
+  </si>
+  <si>
+    <t xml:space="preserve">164 ER 792</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engri0164&amp;i=796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cammell v Sewell (no 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 H&amp;N 578</t>
+  </si>
+  <si>
+    <t xml:space="preserve">157 ER 728</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrh0157&amp;i=1375</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imrie v Castrique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 CB (NS) 405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">141 ER 1222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrg0141&amp;i=1228</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luckmee Chung v Zorawur Mull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 Moo Ind App 291</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 ER 542</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrb0019&amp;i=547</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walker v Hamilton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 De G F&amp;J 602</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45 ER 495</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrc0045&amp;i=503</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burgess v Richardson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29 Beav 478</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54 ER 716</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application of intention, lex loci solutionis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrd0054&amp;i=722</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branley v South Eastern Railway Co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 CB NS 63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">142 ER 1066</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrg0142&amp;i=1070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dutton v Hally</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 B&amp;S 748</t>
+  </si>
+  <si>
+    <t xml:space="preserve">121 ER 1249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrf0121&amp;i=1253</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gardiner v Houghton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 B&amp;S 743</t>
+  </si>
+  <si>
+    <t xml:space="preserve">121 ER 1247</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrf0121&amp;i=1251</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scott v Lord Seymour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 H&amp;C 219</t>
+  </si>
+  <si>
+    <t xml:space="preserve">158 ER 865</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Wild Ranger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lush 552</t>
+  </si>
+  <si>
+    <t xml:space="preserve">167 ER 249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Van Grutten v Digby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 Beav 561</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54 ER 1256</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrd0054&amp;i=1262</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cohen v Gaudet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 F&amp;F 455</t>
+  </si>
+  <si>
+    <t xml:space="preserve">176 ER 204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrk0176&amp;i=208</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In re Hamburg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Moo NS 289</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 ER 911</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrb0015&amp;i=917</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grell v Levy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 CB (NS) 73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">143 ER 1052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrg0143&amp;i=1056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meyer v Dresser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 CB (NS) 646</t>
+  </si>
+  <si>
+    <t xml:space="preserve">143 ER 1280</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrg0143&amp;i=1284</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Bahia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BR &amp; L 292</t>
+  </si>
+  <si>
+    <t xml:space="preserve">167 ER 368</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engri0167&amp;i=372</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lloyd v Guibert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 B&amp;S 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122 ER 1134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://heinonline.org/HOL/P?h=hein.engrep/engrf0122&amp;i=1140</t>
   </si>
 </sst>
 </file>
@@ -3221,6 +3750,22 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0000FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -3291,11 +3836,11 @@
   </sheetPr>
   <dimension ref="A1:M174"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I61" activeCellId="0" sqref="I61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.11"/>
@@ -7887,7 +8432,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -8526,7 +9071,7 @@
       <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="14.84"/>
@@ -8598,11 +9143,11 @@
   </sheetPr>
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -8647,637 +9192,908 @@
     </row>
     <row r="2" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>844</v>
+        <v>1021</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1790</v>
+        <v>1776</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>845</v>
+        <v>1022</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>846</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>847</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>848</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>849</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>850</v>
-      </c>
+        <v>1023</v>
+      </c>
+      <c r="F2" s="4"/>
       <c r="L2" s="0" t="s">
-        <v>851</v>
+        <v>1024</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>852</v>
+        <v>565</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>853</v>
+        <v>1025</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1791</v>
+        <v>1802</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>854</v>
+        <v>1026</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>855</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>856</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>857</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>858</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>859</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>860</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>861</v>
+        <v>1027</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="L3" s="9" t="s">
+        <v>1028</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>1029</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>862</v>
+        <v>1030</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>1795</v>
+        <v>1813</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>863</v>
+        <v>1031</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>864</v>
+        <v>1032</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>856</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>848</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>865</v>
-      </c>
+        <v>604</v>
+      </c>
+      <c r="F4" s="4"/>
       <c r="L4" s="0" t="s">
-        <v>866</v>
+        <v>1033</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>867</v>
+        <v>1034</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>1814</v>
+        <v>1822</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>868</v>
+        <v>1035</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>869</v>
+        <v>1036</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>870</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>871</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>872</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>873</v>
-      </c>
+        <v>262</v>
+      </c>
+      <c r="F5" s="4"/>
       <c r="L5" s="0" t="s">
-        <v>874</v>
+        <v>1037</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>875</v>
+        <v>1038</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>1764</v>
+        <v>1823</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>876</v>
+        <v>1039</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>877</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>878</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>879</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>880</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>881</v>
+        <v>1040</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="0" t="s">
+        <v>373</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>882</v>
+        <v>1041</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>883</v>
+        <v>1042</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1831</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>884</v>
+        <v>1043</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>885</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>604</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>886</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>887</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>879</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>889</v>
-      </c>
+        <v>1044</v>
+      </c>
+      <c r="F7" s="4"/>
       <c r="L7" s="0" t="s">
-        <v>890</v>
+        <v>1045</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>891</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>892</v>
+        <v>1046</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>1814</v>
+        <v>1834</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>893</v>
+        <v>1047</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>894</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>604</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>895</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>896</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>897</v>
-      </c>
-      <c r="K8" s="0" t="s">
-        <v>898</v>
-      </c>
+        <v>1048</v>
+      </c>
+      <c r="F8" s="4"/>
       <c r="L8" s="0" t="s">
-        <v>899</v>
+        <v>1049</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>900</v>
+        <v>1050</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>1749</v>
+        <v>1836</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>901</v>
+        <v>1051</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>902</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>903</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>904</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>879</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>905</v>
-      </c>
-      <c r="K9" s="0" t="s">
-        <v>906</v>
-      </c>
+        <v>1052</v>
+      </c>
+      <c r="F9" s="4"/>
       <c r="L9" s="0" t="s">
-        <v>907</v>
+        <v>1053</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>908</v>
+        <v>1054</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>1801</v>
+        <v>1837</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>909</v>
+        <v>1055</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>910</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>911</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>912</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>913</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>914</v>
-      </c>
-      <c r="L10" s="0" t="s">
-        <v>915</v>
+        <v>1056</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="L10" s="9" t="s">
+        <v>1057</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>916</v>
+        <v>1058</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>1791</v>
+        <v>1840</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>917</v>
+        <v>1059</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>918</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>919</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>858</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>920</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>860</v>
-      </c>
+        <v>1060</v>
+      </c>
+      <c r="F11" s="4"/>
       <c r="L11" s="0" t="s">
-        <v>921</v>
+        <v>1061</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>1062</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>922</v>
+        <v>1063</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>1769</v>
+        <v>1842</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>876</v>
+        <v>1064</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>877</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>923</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>924</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>925</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>926</v>
-      </c>
+        <v>1065</v>
+      </c>
+      <c r="F12" s="4"/>
       <c r="L12" s="0" t="s">
-        <v>882</v>
+        <v>1066</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>927</v>
+        <v>1067</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>1764</v>
+        <v>1842</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>928</v>
+        <v>1068</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>929</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>930</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>931</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>924</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>932</v>
-      </c>
-      <c r="K13" s="0" t="s">
-        <v>860</v>
-      </c>
-      <c r="L13" s="0" t="s">
-        <v>933</v>
+        <v>1069</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="L13" s="9" t="s">
+        <v>1070</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>934</v>
+        <v>1071</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>1787</v>
+        <v>1842</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>935</v>
+        <v>1072</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>936</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>937</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>924</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>938</v>
-      </c>
-      <c r="K14" s="0" t="s">
-        <v>860</v>
-      </c>
+        <v>1073</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="6"/>
       <c r="L14" s="0" t="s">
-        <v>939</v>
+        <v>1074</v>
+      </c>
+      <c r="M14" s="0" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>940</v>
+        <v>1075</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>1826</v>
+        <v>1842</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>941</v>
+        <v>1076</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>942</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>943</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>373</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>944</v>
-      </c>
-      <c r="J15" s="0" t="s">
-        <v>945</v>
-      </c>
-      <c r="K15" s="0" t="s">
-        <v>850</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>946</v>
+        <v>1077</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="L15" s="0" t="s">
+        <v>1078</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>891</v>
+        <v>565</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>947</v>
+        <v>1079</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>1830</v>
+        <v>1843</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>948</v>
+        <v>1080</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>949</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>604</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>950</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>951</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>952</v>
-      </c>
-      <c r="K16" s="0" t="s">
-        <v>850</v>
-      </c>
-      <c r="L16" s="9" t="s">
-        <v>953</v>
+        <v>1081</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="L16" s="0" t="s">
+        <v>1082</v>
+      </c>
+      <c r="M16" s="0" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>954</v>
+        <v>1083</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>1725</v>
+        <v>1846</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>955</v>
+        <v>1084</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>956</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>950</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>951</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>957</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>850</v>
-      </c>
+        <v>1085</v>
+      </c>
+      <c r="F17" s="4"/>
       <c r="L17" s="0" t="s">
-        <v>958</v>
+        <v>1086</v>
+      </c>
+      <c r="M17" s="0" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>959</v>
+        <v>1087</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>1831</v>
+        <v>1850</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>960</v>
+        <v>1088</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>961</v>
+        <v>1089</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>962</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>963</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>964</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>965</v>
-      </c>
+      <c r="F18" s="4"/>
       <c r="L18" s="0" t="s">
-        <v>966</v>
+        <v>1090</v>
+      </c>
+      <c r="M18" s="0" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>1850</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>1093</v>
+      </c>
       <c r="F19" s="4"/>
+      <c r="L19" s="0" t="s">
+        <v>1094</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>1853</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>1097</v>
+      </c>
       <c r="F20" s="4"/>
+      <c r="L20" s="0" t="s">
+        <v>1098</v>
+      </c>
+      <c r="M20" s="0" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F21" s="4"/>
+      <c r="A21" s="0" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>1854</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>1100</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>1101</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>1102</v>
+      </c>
+      <c r="L21" s="0" t="s">
+        <v>1103</v>
+      </c>
+      <c r="M21" s="0" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>1855</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>1106</v>
+      </c>
       <c r="F22" s="4"/>
+      <c r="L22" s="0" t="s">
+        <v>1107</v>
+      </c>
+      <c r="M22" s="0" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>1858</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>1110</v>
+      </c>
       <c r="F23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="6"/>
+      <c r="L23" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="M23" s="0" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>1858</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>1114</v>
+      </c>
       <c r="F24" s="4"/>
+      <c r="K24" s="0" t="s">
+        <v>1115</v>
+      </c>
+      <c r="L24" s="0" t="s">
+        <v>1116</v>
+      </c>
+      <c r="M24" s="0" t="s">
+        <v>557</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>1858</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>1119</v>
+      </c>
       <c r="F25" s="4"/>
+      <c r="L25" s="0" t="s">
+        <v>1120</v>
+      </c>
+      <c r="M25" s="0" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>1859</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>1123</v>
+      </c>
       <c r="F26" s="4"/>
+      <c r="L26" s="0" t="s">
+        <v>1124</v>
+      </c>
+      <c r="M26" s="0" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>1860</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>1127</v>
+      </c>
       <c r="F27" s="4"/>
+      <c r="L27" s="0" t="s">
+        <v>1128</v>
+      </c>
+      <c r="M27" s="0" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>1860</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>1131</v>
+      </c>
       <c r="F28" s="4"/>
+      <c r="L28" s="9" t="s">
+        <v>1132</v>
+      </c>
+      <c r="M28" s="0" t="s">
+        <v>557</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>1860</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>1135</v>
+      </c>
       <c r="F29" s="4"/>
+      <c r="L29" s="0" t="s">
+        <v>1136</v>
+      </c>
+      <c r="M29" s="0" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>1860</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>1139</v>
+      </c>
       <c r="F30" s="4"/>
+      <c r="L30" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="M30" s="0" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F31" s="4"/>
+      <c r="A31" s="0" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>1861</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>1143</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>1144</v>
+      </c>
+      <c r="L31" s="0" t="s">
+        <v>1145</v>
+      </c>
+      <c r="M31" s="0" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>1862</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>1148</v>
+      </c>
       <c r="F32" s="4"/>
+      <c r="L32" s="9" t="s">
+        <v>1149</v>
+      </c>
+      <c r="M32" s="0" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>1862</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>1151</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>1152</v>
+      </c>
       <c r="F33" s="4"/>
+      <c r="L33" s="0" t="s">
+        <v>1153</v>
+      </c>
+      <c r="M33" s="0" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>1862</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>1156</v>
+      </c>
       <c r="F34" s="4"/>
+      <c r="L34" s="0" t="s">
+        <v>1157</v>
+      </c>
+      <c r="M34" s="0" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>1862</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>1159</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>1160</v>
+      </c>
       <c r="F35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="M35" s="0" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>1862</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>1162</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>1163</v>
+      </c>
       <c r="F36" s="4"/>
+      <c r="L36" s="0" t="s">
+        <v>1098</v>
+      </c>
+      <c r="M36" s="0" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F37" s="4"/>
+      <c r="A37" s="0" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>1862</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>1166</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>1062</v>
+      </c>
+      <c r="L37" s="0" t="s">
+        <v>1167</v>
+      </c>
+      <c r="M37" s="0" t="s">
+        <v>801</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>1863</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>1169</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>1170</v>
+      </c>
       <c r="F38" s="4"/>
+      <c r="L38" s="0" t="s">
+        <v>1171</v>
+      </c>
+      <c r="M38" s="0" t="s">
+        <v>801</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>1863</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>1173</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>1174</v>
+      </c>
       <c r="F39" s="4"/>
+      <c r="L39" s="9" t="s">
+        <v>1175</v>
+      </c>
+      <c r="M39" s="0" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>1864</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>1178</v>
+      </c>
       <c r="F40" s="4"/>
+      <c r="L40" s="0" t="s">
+        <v>1179</v>
+      </c>
+      <c r="M40" s="0" t="s">
+        <v>801</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>1864</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>1182</v>
+      </c>
       <c r="F41" s="4"/>
+      <c r="L41" s="0" t="s">
+        <v>1183</v>
+      </c>
+      <c r="M41" s="0" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>1864</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>1186</v>
+      </c>
       <c r="F42" s="4"/>
+      <c r="L42" s="0" t="s">
+        <v>1187</v>
+      </c>
+      <c r="M42" s="0" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>1865</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>1190</v>
+      </c>
       <c r="F43" s="4"/>
+      <c r="L43" s="0" t="s">
+        <v>1191</v>
+      </c>
+      <c r="M43" s="0" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F44" s="4"/>
@@ -9393,8 +10209,10 @@
     <row r="143" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L15" r:id="rId1" display="https://heinonline.org/HOL/P?h=hein.engrep/engrf0108&amp;i=167"/>
-    <hyperlink ref="L16" r:id="rId2" display="https://heinonline.org/HOL/P?h=hein.engrep/engra0006&amp;i=769"/>
+    <hyperlink ref="L3" r:id="rId1" display="https://heinonline.org/HOL/P?h=hein.engrep/engri0161&amp;i=803"/>
+    <hyperlink ref="L10" r:id="rId2" display="https://heinonline.org/HOL/P?h=hein.engrep/engrf0112&amp;i=74"/>
+    <hyperlink ref="L13" r:id="rId3" display="https://heinonline.org/HOL/P?h=hein"/>
+    <hyperlink ref="L39" r:id="rId4" display="https://heinonline.org/HOL/P?h=hein.engrep/engrb0015&amp;i=917"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>